<commit_message>
{{ mustache }} syntax
Conditional row output (CASE)
In MS Word .docx format deleting tags between chars in fields' search
;func%3DSUM|AVG|COUNT|FISRT
</commit_message>
<xml_diff>
--- a/src/zxxt_05_excel_xlsx.w3mi.data.xlsx
+++ b/src/zxxt_05_excel_xlsx.w3mi.data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\modek\Desktop\XTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>{R-TITLE}</t>
   </si>
@@ -42,33 +42,18 @@
     <t>---------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------</t>
   </si>
   <si>
-    <t xml:space="preserve">Totals for all groups </t>
-  </si>
-  <si>
     <t>Groups count {R-T-CH_COUNT}</t>
   </si>
   <si>
     <t>{R-T-SUM1}</t>
   </si>
   <si>
-    <t>{R-T-SUM2}</t>
-  </si>
-  <si>
     <t>{R-T;level=1;top=X}</t>
   </si>
   <si>
-    <t xml:space="preserve">Sub totals of group {R-T-GROUP} </t>
-  </si>
-  <si>
-    <t>Sub items count {R-T-CH_COUNT}</t>
-  </si>
-  <si>
     <t>{R-T;level=1;top=}</t>
   </si>
   <si>
-    <t xml:space="preserve">End of {R-T-GROUP} </t>
-  </si>
-  <si>
     <t>{R-T;level=2;top=X}</t>
   </si>
   <si>
@@ -76,13 +61,70 @@
   </si>
   <si>
     <t>{R-T-GROUP}</t>
+  </si>
+  <si>
+    <t>{R-T;level=1;top=X;show_if=ROW-GROUP eq 'GRP B'}</t>
+  </si>
+  <si>
+    <t>DEFAULT header (WHEN OTHERS)</t>
+  </si>
+  <si>
+    <t>Footer is the same</t>
+  </si>
+  <si>
+    <t>Complex where with ()</t>
+  </si>
+  <si>
+    <t>{R-T;level=1;top=X;hide_if=row-GROUP = 'GRP D'}</t>
+  </si>
+  <si>
+    <t>{R-T;level=1;top=X;show_if=( row-GROUP = 'C' OR ROW-group cp '*C' ) AND ROW-GROUP &lt;&gt; 'Z' }</t>
+  </si>
+  <si>
+    <t>Sub items count {R-T-CH_COUNT;func=COUNT}</t>
+  </si>
+  <si>
+    <t>{R-T-SUM1;func=SUM}</t>
+  </si>
+  <si>
+    <t>{R-T-SUM2;func=SUM}</t>
+  </si>
+  <si>
+    <t>{R-T-SUM1;func=AVG}</t>
+  </si>
+  <si>
+    <t>{R-T-SUM2;func=AVG}</t>
+  </si>
+  <si>
+    <t>COUNT = {R-T-CH_COUNT;func=COUNT}</t>
+  </si>
+  <si>
+    <t>COUNT= {R-T-CH_COUNT}</t>
+  </si>
+  <si>
+    <t>Average for SUM1 &amp; SUM2</t>
+  </si>
+  <si>
+    <t>Group {R-T-GROUP;func=FIRST}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group {R-T-GROUP} </t>
+  </si>
+  <si>
+    <t>End of {R-T-GROUP} sum for SUM1 &amp; SUM2</t>
+  </si>
+  <si>
+    <t>Header for GROUP 'B' 2 rows</t>
+  </si>
+  <si>
+    <t>Do not show header for 'D' group! (hide_if=)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -234,8 +276,23 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -423,18 +480,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF2E74B5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF9CC2E5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -627,19 +708,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -663,6 +731,63 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -710,7 +835,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -722,39 +847,52 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="34" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="36" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="34" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="36" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="35" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="37" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -765,6 +903,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="35" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="35" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="35" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="35" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -866,7 +1031,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -918,7 +1083,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1119,132 +1284,198 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="3" max="3" width="41.85546875" customWidth="1"/>
-    <col min="4" max="6" width="33.42578125" customWidth="1"/>
-    <col min="7" max="7" width="30.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="46" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" customWidth="1"/>
+    <col min="5" max="7" width="33.42578125" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="1"/>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="C4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="4"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="E5" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="31"/>
+      <c r="F7" s="33"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="34"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="13"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>9</v>
+      <c r="F13" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B4:E4"/>
+  <mergeCells count="6">
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>